<commit_message>
Sprint : PPG Sprint 3    state :inProgress
</commit_message>
<xml_diff>
--- a/Unit_10_SecondTermProject/ECU2/TestCases/ECU2_AdminDashboard.xlsx
+++ b/Unit_10_SecondTermProject/ECU2/TestCases/ECU2_AdminDashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\COURSES\Learn-in-Depth\FullProject\ECU2\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F627AF-9E1F-45BA-A19E-7D3E1F75F3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B08BE8-CAD1-42B8-AE0D-021F11D1E10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FBA70518-CB10-42FD-A195-A863F06D5FAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="89">
   <si>
     <t>Test ID</t>
   </si>
@@ -251,9 +251,6 @@
     <t>MCU Read 5</t>
   </si>
   <si>
-    <t>onGoing</t>
-  </si>
-  <si>
     <t>Validate functionality of BCD seven Segment
  (ECU3)</t>
   </si>
@@ -306,23 +303,62 @@
     <t>"Hello World!"</t>
   </si>
   <si>
-    <t>gotoLine(1,2)
+    <t>clearScreen()</t>
+  </si>
+  <si>
+    <t>noOutput</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print star ('|_|') </t>
+  </si>
+  <si>
+    <t>|_|</t>
+  </si>
+  <si>
+    <t>Ahleen @x=16  y=0
+Ahleen @x=16  y=1
+Ahleen @x=16  y=2
+Ahleen @x=16  y=3</t>
+  </si>
+  <si>
+    <t>gotoLine(16,0)
+write("Ahleen")
+gotoLine(16,1)
+write("Ahleen")
+gotoLine(16,2)
+write("Ahleen")
+gotoLine(16,3)
 write("Ahleen")</t>
   </si>
   <si>
-    <t>Ahleen @x=1  y=2</t>
-  </si>
-  <si>
-    <t>clearScreen()</t>
-  </si>
-  <si>
-    <t>noOutput</t>
-  </si>
-  <si>
-    <t xml:space="preserve">print star ('|_|') </t>
-  </si>
-  <si>
-    <t>|_|</t>
+    <t>Ahleen @x=16  y=0
+Ahleen @x=16  y=1
+Ahleen @x=16  y=2
+Ahleen @x=16  y=4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate functionality of SPI Communication
+ (ECU3) </t>
+  </si>
+  <si>
+    <t>TC_SPI_15</t>
+  </si>
+  <si>
+    <t>Validate that the can exchange data by SPI</t>
+  </si>
+  <si>
+    <t>1-STM32CUBE IDE 
+2- Proteus Simulation
+3- RCC Driver 
+4- GPIO Driver
+5- SPI</t>
+  </si>
+  <si>
+    <t>Exchange '+' and 'A' between master and slave</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'a' at master
+'+' at slave</t>
   </si>
 </sst>
 </file>
@@ -407,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -422,26 +458,11 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -453,16 +474,228 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
+  <dxfs count="144">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2015,13 +2248,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB1C29D-A9BC-4A81-B2AF-DC978394A8D6}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="129" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="129" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="17" customWidth="1"/>
+    <col min="1" max="1" width="18" style="11" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" hidden="1" customWidth="1"/>
@@ -2037,7 +2270,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2075,7 +2308,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
@@ -2108,10 +2341,10 @@
       <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="6"/>
+      <c r="M2" s="12"/>
     </row>
     <row r="3" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
+      <c r="A3" s="15"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -2142,10 +2375,10 @@
       <c r="L3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="7"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -2176,10 +2409,10 @@
       <c r="L4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="7"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -2210,10 +2443,10 @@
       <c r="L5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="7"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -2244,10 +2477,10 @@
       <c r="L6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="7"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2262,7 +2495,7 @@
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B8" t="s">
@@ -2297,7 +2530,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>44</v>
       </c>
@@ -2330,7 +2563,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2345,8 +2578,8 @@
       <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>62</v>
+      <c r="A11" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>55</v>
@@ -2380,7 +2613,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2395,8 +2628,8 @@
       <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>63</v>
+      <c r="A13" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B13" t="s">
         <v>56</v>
@@ -2430,7 +2663,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2445,26 +2678,26 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="E15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>14</v>
@@ -2480,24 +2713,27 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
+      <c r="A16" s="15"/>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="8">
-        <v>100</v>
-      </c>
-      <c r="G16" s="9">
-        <v>100</v>
+        <v>74</v>
+      </c>
+      <c r="F16" s="6">
+        <v>123123001</v>
+      </c>
+      <c r="G16" s="7">
+        <v>123123001</v>
+      </c>
+      <c r="H16">
+        <v>123123001</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>12</v>
@@ -2509,24 +2745,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" t="s">
-        <v>78</v>
+        <v>81</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>12</v>
@@ -2538,24 +2778,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>14</v>
@@ -2570,25 +2811,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+    <row r="19" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="F19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="H19" t="s">
+        <v>77</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>12</v>
@@ -2600,132 +2844,279 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C20" s="2"/>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F26" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="M2:M6"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A15:A19"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A1:M1 F26 A7:M7 A10:M10 A2:B2 A3:C6 C6:D6 D4:D5 E2:E6 D2:M3 F4:M6 A8:E8 B9:G9 F8:L9 B11:C11 B15:B20">
-    <cfRule type="cellIs" dxfId="123" priority="165" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="166" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="167" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="168" operator="equal">
+  <conditionalFormatting sqref="A1:M1 F26 A7:M7 A10:M10 A2:B2 A3:C6 C6:D6 D4:D5 E2:E6 D2:M3 F4:M6 A8:E8 B9:G9 F8:L9 B11:C11 B15:B19 B21">
+    <cfRule type="cellIs" dxfId="143" priority="201" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="202" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="203" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="204" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="115" priority="137" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="138" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="139" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="173" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="174" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="175" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="176" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:H11">
-    <cfRule type="cellIs" dxfId="111" priority="133" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="134" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="135" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="169" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="170" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="171" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="172" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="107" priority="129" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="130" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="131" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="165" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="166" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="167" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="168" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="103" priority="125" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="126" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="127" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="161" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="162" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="163" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="164" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="99" priority="121" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="122" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="123" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="157" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="158" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="159" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="160" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:M12">
-    <cfRule type="cellIs" dxfId="95" priority="117" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="118" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="119" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="153" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="154" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="155" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="156" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="cellIs" dxfId="91" priority="105" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="106" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="107" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="141" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="142" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="143" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="144" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13 F15:F16">
+    <cfRule type="cellIs" dxfId="111" priority="125" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="126" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="109" priority="127" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="128" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13 I15:I19">
+    <cfRule type="cellIs" dxfId="107" priority="121" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="122" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="123" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="124" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" dxfId="103" priority="109" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="110" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="111" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="112" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="cellIs" dxfId="99" priority="105" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="106" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13">
+    <cfRule type="cellIs" dxfId="95" priority="101" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="102" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="103" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="104" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="91" priority="97" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="98" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="99" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="100" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
     <cfRule type="cellIs" dxfId="87" priority="89" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2739,7 +3130,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13 I15:I19">
+  <conditionalFormatting sqref="L13">
     <cfRule type="cellIs" dxfId="83" priority="85" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2753,91 +3144,119 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="75" priority="73" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="74" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="76" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="71" priority="69" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="70" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="71" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="67" priority="65" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="66" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="62" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="63" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="64" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="55" priority="53" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="56" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L11">
+    <cfRule type="cellIs" dxfId="79" priority="81" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="82" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="83" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="84" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="cellIs" dxfId="75" priority="77" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="78" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="79" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="80" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="cellIs" dxfId="71" priority="73" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="74" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="75" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="76" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:M14">
+    <cfRule type="cellIs" dxfId="67" priority="69" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="70" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="71" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="72" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="cellIs" dxfId="63" priority="65" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="67" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="68" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:C19">
+    <cfRule type="cellIs" dxfId="59" priority="61" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="62" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="63" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15:E19">
+    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="58" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="60" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15:H15">
+    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="56" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L15:L19">
     <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2851,7 +3270,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
+  <conditionalFormatting sqref="J15:J19">
     <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2865,7 +3284,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
+  <conditionalFormatting sqref="K15:K19">
     <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2879,7 +3298,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:M14">
+  <conditionalFormatting sqref="A20:M20">
     <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2893,7 +3312,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
+  <conditionalFormatting sqref="A21">
     <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2907,7 +3326,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C20">
+  <conditionalFormatting sqref="C21">
     <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2921,7 +3340,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E19">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2935,7 +3354,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G15:H15">
+  <conditionalFormatting sqref="I21">
     <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2949,7 +3368,21 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L15:L19">
+  <conditionalFormatting sqref="J21">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2963,7 +3396,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J15:J19">
+  <conditionalFormatting sqref="L21">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -2977,7 +3410,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K15:K19">
+  <conditionalFormatting sqref="A22:M22">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Sprint : PPG Sprint 3    state :Finished
</commit_message>
<xml_diff>
--- a/Unit_10_SecondTermProject/ECU2/TestCases/ECU2_AdminDashboard.xlsx
+++ b/Unit_10_SecondTermProject/ECU2/TestCases/ECU2_AdminDashboard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\COURSES\Learn-in-Depth\FullProject\ECU2\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\COURSES\Learn-in-Depth\Repo\Unit_10_SecondTermProject\ECU2\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B08BE8-CAD1-42B8-AE0D-021F11D1E10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E84F58-36AF-44CC-B8F1-FE46CF642A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FBA70518-CB10-42FD-A195-A863F06D5FAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="98">
   <si>
     <t>Test ID</t>
   </si>
@@ -359,6 +359,39 @@
   <si>
     <t xml:space="preserve"> 'a' at master
 '+' at slave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate functionality of EEPROM
+ (ECU3) </t>
+  </si>
+  <si>
+    <t>TC_EEPROM_16</t>
+  </si>
+  <si>
+    <t>TC_EEPROM_17</t>
+  </si>
+  <si>
+    <t>Validate that the can store data on eeprom</t>
+  </si>
+  <si>
+    <t>Validate that the can get data from eeprom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-STM32CUBE IDE 
+2- Proteus Simulation
+3- RCC Driver 
+4- GPIO Driver
+5- SPI
+</t>
+  </si>
+  <si>
+    <t>store A @ 0x00FF</t>
+  </si>
+  <si>
+    <t>Get data @ 0x00FF</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -443,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -476,6 +509,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,14 +524,2064 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="144">
+  <dxfs count="349">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2248,8 +4334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB1C29D-A9BC-4A81-B2AF-DC978394A8D6}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="129" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="129" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2308,7 +4394,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
@@ -2341,10 +4427,10 @@
       <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="12"/>
+      <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
+      <c r="A3" s="16"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -2375,10 +4461,10 @@
       <c r="L3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="13"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="16"/>
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -2409,10 +4495,10 @@
       <c r="L4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="13"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -2443,10 +4529,10 @@
       <c r="L5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="13"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -2477,7 +4563,7 @@
       <c r="L6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="13"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
@@ -2495,7 +4581,7 @@
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B8" t="s">
@@ -2530,7 +4616,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" t="s">
         <v>44</v>
       </c>
@@ -2678,7 +4764,7 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B15" t="s">
@@ -2713,7 +4799,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
+      <c r="A16" s="16"/>
       <c r="B16" t="s">
         <v>66</v>
       </c>
@@ -2746,7 +4832,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
+      <c r="A17" s="16"/>
       <c r="B17" t="s">
         <v>67</v>
       </c>
@@ -2779,7 +4865,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
+      <c r="A18" s="16"/>
       <c r="B18" t="s">
         <v>68</v>
       </c>
@@ -2812,7 +4898,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="16"/>
       <c r="B19" t="s">
         <v>69</v>
       </c>
@@ -2875,10 +4961,10 @@
       <c r="F21" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="12" t="s">
         <v>88</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -2894,7 +4980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2909,424 +4995,647 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
+    <row r="23" spans="1:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" t="s">
+        <v>97</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+    </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F26" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="M2:M6"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A23:A24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A1:M1 F26 A7:M7 A10:M10 A2:B2 A3:C6 C6:D6 D4:D5 E2:E6 D2:M3 F4:M6 A8:E8 B9:G9 F8:L9 B11:C11 B15:B19 B21">
-    <cfRule type="cellIs" dxfId="143" priority="201" operator="equal">
+  <conditionalFormatting sqref="A1:M1 F26 A7:M7 A10:M10 A2:B2 A3:C6 C6:D6 D4:D5 E2:E6 D2:M3 F4:M6 A8:E8 B9:G9 F8:L9 B11:C11 B15:B19 B21 B23:B24">
+    <cfRule type="cellIs" dxfId="348" priority="250" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="251" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="346" priority="252" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="345" priority="253" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="139" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="222" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="343" priority="223" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="342" priority="224" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="225" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:H11">
-    <cfRule type="cellIs" dxfId="135" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="340" priority="218" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="339" priority="219" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="220" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="337" priority="221" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="131" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="336" priority="214" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="215" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="334" priority="216" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="333" priority="217" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="127" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="210" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="331" priority="211" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="330" priority="212" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="213" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="123" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="328" priority="206" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="327" priority="207" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="208" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="325" priority="209" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:M12">
-    <cfRule type="cellIs" dxfId="119" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="324" priority="202" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="203" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="322" priority="204" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="321" priority="205" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="cellIs" dxfId="115" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="190" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="319" priority="191" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="318" priority="192" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="193" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13 F15:F16">
-    <cfRule type="cellIs" dxfId="111" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="316" priority="174" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="315" priority="175" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="176" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="313" priority="177" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13 I15:I19">
-    <cfRule type="cellIs" dxfId="107" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="312" priority="170" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="171" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="310" priority="172" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="309" priority="173" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="103" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="158" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="307" priority="159" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="306" priority="160" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="161" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="99" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="304" priority="154" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="303" priority="155" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="156" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="301" priority="157" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="95" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="300" priority="150" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="151" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="298" priority="152" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="297" priority="153" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="91" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="146" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="295" priority="147" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="294" priority="148" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="149" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="87" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="292" priority="138" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="291" priority="139" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="140" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="289" priority="141" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="83" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="288" priority="134" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="135" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="286" priority="136" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="285" priority="137" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="cellIs" dxfId="79" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="130" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="283" priority="131" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="282" priority="132" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="133" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="75" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="280" priority="126" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="279" priority="127" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="128" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="277" priority="129" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="71" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="276" priority="122" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="123" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="274" priority="124" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="273" priority="125" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:M14">
-    <cfRule type="cellIs" dxfId="67" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="118" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="271" priority="119" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="270" priority="120" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="121" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="63" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="114" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="267" priority="115" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="116" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="265" priority="117" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C19">
-    <cfRule type="cellIs" dxfId="59" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="264" priority="110" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="111" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="262" priority="112" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="261" priority="113" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E19">
-    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="106" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="107" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="108" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="109" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:H15">
-    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="102" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="103" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="104" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="105" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:L19">
-    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="94" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="95" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="96" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="97" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J19">
-    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="90" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="91" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="92" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="93" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:K19">
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="86" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="87" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="88" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="89" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:M20">
-    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="82" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="83" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="84" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="85" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="78" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="79" operator="equal">
       <formula>"onGoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="80" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="81" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
+    <cfRule type="cellIs" dxfId="232" priority="74" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="231" priority="75" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="230" priority="76" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="229" priority="77" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="228" priority="70" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="227" priority="71" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="72" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="225" priority="73" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
+    <cfRule type="cellIs" dxfId="224" priority="66" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="223" priority="67" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="222" priority="68" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="221" priority="69" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21">
+    <cfRule type="cellIs" dxfId="220" priority="62" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="219" priority="63" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="218" priority="64" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="65" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="cellIs" dxfId="216" priority="58" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="215" priority="59" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="60" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="213" priority="61" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L21">
+    <cfRule type="cellIs" dxfId="212" priority="54" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="55" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="210" priority="56" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="209" priority="57" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:M22">
+    <cfRule type="cellIs" dxfId="208" priority="50" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="207" priority="51" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="206" priority="52" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="205" priority="53" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="cellIs" dxfId="204" priority="46" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="203" priority="47" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="202" priority="48" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="201" priority="49" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:C24">
+    <cfRule type="cellIs" dxfId="200" priority="42" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="199" priority="43" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="198" priority="44" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="197" priority="45" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:E24">
+    <cfRule type="cellIs" dxfId="196" priority="30" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="195" priority="31" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="194" priority="32" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="33" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I23:I24">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:M25">
     <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -3340,7 +5649,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="J23">
     <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -3354,7 +5663,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
+  <conditionalFormatting sqref="J24">
     <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -3368,7 +5677,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J21">
+  <conditionalFormatting sqref="K23">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -3382,7 +5691,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
+  <conditionalFormatting sqref="K24">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -3396,7 +5705,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L21">
+  <conditionalFormatting sqref="L23">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -3410,7 +5719,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A22:M22">
+  <conditionalFormatting sqref="L24">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Sprint : PPG Sprint 4    state : inProgress
</commit_message>
<xml_diff>
--- a/Unit_10_SecondTermProject/ECU2/TestCases/ECU2_AdminDashboard.xlsx
+++ b/Unit_10_SecondTermProject/ECU2/TestCases/ECU2_AdminDashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\COURSES\Learn-in-Depth\Repo\Unit_10_SecondTermProject\ECU2\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6A87B8-AC98-436E-81BB-531B78D431D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8057E214-EFE6-40BB-9062-DF469B30881E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FBA70518-CB10-42FD-A195-A863F06D5FAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="126">
   <si>
     <t>Test ID</t>
   </si>
@@ -464,6 +464,44 @@
   </si>
   <si>
     <t>Display Adding screen</t>
+  </si>
+  <si>
+    <t>TC_ADMIN_22</t>
+  </si>
+  <si>
+    <t>TC_ADMIN_23</t>
+  </si>
+  <si>
+    <t>TC_ADMIN_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that Admin Can Delete Driver </t>
+  </si>
+  <si>
+    <t>Admin Data
+username: "Mohamed"
+Pasword: "000001"
+No Exist Driver</t>
+  </si>
+  <si>
+    <t>Display Unsuccessful</t>
+  </si>
+  <si>
+    <t>Admin Data
+username: "Mohamed"
+Driver Data
+"MoSalh"
+"1234567"</t>
+  </si>
+  <si>
+    <t>Admin Data
+username: "Mohamed"
+Driver Data
+"MoSalah"
+"1234567"</t>
+  </si>
+  <si>
+    <t>Display Successful</t>
   </si>
 </sst>
 </file>
@@ -585,16 +623,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -646,461 +684,461 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2934,10 +2972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB1C29D-A9BC-4A81-B2AF-DC978394A8D6}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="129" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2951,7 +2989,7 @@
     <col min="7" max="7" width="23.140625" customWidth="1"/>
     <col min="8" max="8" width="24.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
     <col min="12" max="12" width="15.140625" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
@@ -2996,7 +3034,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
@@ -3029,10 +3067,10 @@
       <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="15"/>
+      <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+      <c r="A3" s="16"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -3063,10 +3101,10 @@
       <c r="L3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="16"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
+      <c r="A4" s="16"/>
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -3097,10 +3135,10 @@
       <c r="L4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="16"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="16"/>
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -3131,10 +3169,10 @@
       <c r="L5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="16"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="16"/>
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -3165,7 +3203,7 @@
       <c r="L6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="16"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
@@ -3183,7 +3221,7 @@
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B8" t="s">
@@ -3218,7 +3256,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="16"/>
       <c r="B9" t="s">
         <v>44</v>
       </c>
@@ -3366,7 +3404,7 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B15" t="s">
@@ -3401,7 +3439,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
+      <c r="A16" s="16"/>
       <c r="B16" t="s">
         <v>66</v>
       </c>
@@ -3434,7 +3472,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="16"/>
       <c r="B17" t="s">
         <v>67</v>
       </c>
@@ -3467,7 +3505,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
+      <c r="A18" s="16"/>
       <c r="B18" t="s">
         <v>68</v>
       </c>
@@ -3500,7 +3538,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="16"/>
       <c r="B19" t="s">
         <v>69</v>
       </c>
@@ -3598,7 +3636,7 @@
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="15" t="s">
         <v>89</v>
       </c>
       <c r="B23" t="s">
@@ -3630,7 +3668,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="16"/>
       <c r="B24" t="s">
         <v>91</v>
       </c>
@@ -3675,7 +3713,7 @@
       <c r="M25" s="5"/>
     </row>
     <row r="26" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="15" t="s">
         <v>112</v>
       </c>
       <c r="B26" t="s">
@@ -3775,7 +3813,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" t="s">
         <v>113</v>
@@ -3808,723 +3846,826 @@
         <v>111</v>
       </c>
     </row>
+    <row r="30" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I31" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I32" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="2"/>
+      <c r="E33" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A26:A32"/>
     <mergeCell ref="M2:M6"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A15:A19"/>
     <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A26:A29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A1:M1 A7:M7 A10:M10 A2:B2 A3:C6 C6:D6 D4:D5 E2:E6 D2:M3 F4:M6 A8:E8 B9:G9 F8:L9 B11:C11 B15:B19 B21 B23:B24 B26:B29 F26:F29">
-    <cfRule type="cellIs" dxfId="3" priority="267" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="268" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="269" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="270" operator="equal">
+  <conditionalFormatting sqref="A1:M1 A7:M7 A10:M10 A2:B2 A3:C6 C6:D6 D4:D5 E2:E6 D2:M3 F4:M6 A8:E8 B9:G9 F8:L9 B11:C11 B15:B19 B21 B23:B24 B26:B34 F26:F32">
+    <cfRule type="cellIs" dxfId="201" priority="267" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="200" priority="268" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="199" priority="269" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="198" priority="270" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="201" priority="239" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="240" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="199" priority="241" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="242" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="239" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="240" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="195" priority="241" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="194" priority="242" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:H11">
-    <cfRule type="cellIs" dxfId="197" priority="235" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="236" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="195" priority="237" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="238" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="235" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="192" priority="236" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="191" priority="237" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="238" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="193" priority="231" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="232" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="233" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="231" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="188" priority="232" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="187" priority="233" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="186" priority="234" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="189" priority="227" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="228" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="229" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="227" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="184" priority="228" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="183" priority="229" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="182" priority="230" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="185" priority="223" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="224" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="225" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="223" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="180" priority="224" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="179" priority="225" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="178" priority="226" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:M12">
-    <cfRule type="cellIs" dxfId="181" priority="219" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="220" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="221" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="219" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="220" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="175" priority="221" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="174" priority="222" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="cellIs" dxfId="177" priority="207" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="208" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="209" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="207" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="172" priority="208" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="171" priority="209" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="170" priority="210" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13 F15:F16">
-    <cfRule type="cellIs" dxfId="173" priority="191" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="192" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="193" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="191" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="168" priority="192" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="167" priority="193" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="194" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13 I15:I19">
-    <cfRule type="cellIs" dxfId="169" priority="187" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="188" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="189" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="187" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="188" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="163" priority="189" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="162" priority="190" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="165" priority="175" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="176" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="177" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="175" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="176" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="159" priority="177" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="178" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="161" priority="171" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="172" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="173" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="171" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="156" priority="172" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="173" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="174" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="157" priority="167" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="168" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="169" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="167" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="152" priority="168" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="169" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="170" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="153" priority="163" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="164" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="165" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="163" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="164" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="165" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="166" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="149" priority="155" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="156" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="157" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="155" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="156" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="143" priority="157" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="158" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="145" priority="151" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="152" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="153" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="151" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="152" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="139" priority="153" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="154" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="cellIs" dxfId="141" priority="147" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="148" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="149" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="147" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="148" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="135" priority="149" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="150" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="cellIs" dxfId="137" priority="143" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="144" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="145" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="143" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="144" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="145" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="146" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="133" priority="139" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="140" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="141" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="139" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="140" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="141" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="142" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:M14">
-    <cfRule type="cellIs" dxfId="129" priority="135" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="136" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="137" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="135" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="136" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="137" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="138" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="125" priority="131" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="132" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="133" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="131" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="132" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="133" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="134" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:C19">
-    <cfRule type="cellIs" dxfId="121" priority="127" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="128" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="129" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="127" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="128" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="129" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="130" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15:E19">
-    <cfRule type="cellIs" dxfId="117" priority="123" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="124" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="125" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="123" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="124" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="111" priority="125" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="126" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:H15">
-    <cfRule type="cellIs" dxfId="113" priority="119" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="120" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="121" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="119" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="120" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="121" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="122" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:L19">
-    <cfRule type="cellIs" dxfId="109" priority="111" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="112" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="113" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="111" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="112" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="103" priority="113" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="114" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:J19">
-    <cfRule type="cellIs" dxfId="105" priority="107" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="108" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="109" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="107" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="108" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="109" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="110" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:K19">
-    <cfRule type="cellIs" dxfId="101" priority="103" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="104" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="105" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="103" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="104" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="105" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="106" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:M20">
-    <cfRule type="cellIs" dxfId="97" priority="99" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="100" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="101" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="99" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="100" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="101" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="102" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="93" priority="95" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="96" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="97" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="95" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="96" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="97" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="98" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="89" priority="91" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="92" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="93" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="91" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="92" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="83" priority="93" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="94" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="85" priority="87" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="88" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="89" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="87" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="88" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="89" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="90" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="cellIs" dxfId="81" priority="83" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="85" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="83" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="84" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="85" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="86" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21">
-    <cfRule type="cellIs" dxfId="77" priority="79" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="80" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="81" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="79" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="80" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="81" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="82" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="73" priority="75" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="76" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="77" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="75" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="76" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="77" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="78" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="cellIs" dxfId="69" priority="71" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="73" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="71" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="72" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="73" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="74" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:M22">
-    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="68" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="69" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="67" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="68" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="69" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="70" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="cellIs" dxfId="61" priority="63" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="64" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="65" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="63" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="65" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="66" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:C24">
-    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="60" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="61" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="62" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E24">
-    <cfRule type="cellIs" dxfId="53" priority="47" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="48" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I24">
-    <cfRule type="cellIs" dxfId="49" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:M25">
-    <cfRule type="cellIs" dxfId="48" priority="42" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="43" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="44" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23">
-    <cfRule type="cellIs" dxfId="44" priority="38" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="39" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24">
-    <cfRule type="cellIs" dxfId="40" priority="34" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="35" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="36" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="36" priority="30" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="31" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="32" priority="26" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24">
-    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="20" priority="14" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C29">
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E29">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C33">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:E33">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>$I$27</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J26:L29">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+  <conditionalFormatting sqref="J26:L32">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Sprint : PPG Sprint 5    state : inProgress
</commit_message>
<xml_diff>
--- a/Unit_10_SecondTermProject/ECU2/TestCases/ECU2_AdminDashboard.xlsx
+++ b/Unit_10_SecondTermProject/ECU2/TestCases/ECU2_AdminDashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\COURSES\Learn-in-Depth\Repo\Unit_10_SecondTermProject\ECU2\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8057E214-EFE6-40BB-9062-DF469B30881E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CABBF5-D43A-4CE1-B413-5C61EE997BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FBA70518-CB10-42FD-A195-A863F06D5FAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="143">
   <si>
     <t>Test ID</t>
   </si>
@@ -502,6 +502,76 @@
   </si>
   <si>
     <t>Display Successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate functionality of EXTI
+ (ECU3) </t>
+  </si>
+  <si>
+    <t>TC_EXTI_25</t>
+  </si>
+  <si>
+    <t>TC_EXTI_26</t>
+  </si>
+  <si>
+    <t>TC_EXTI_27</t>
+  </si>
+  <si>
+    <t>Validate that EXTI 1 Works on any logic change</t>
+  </si>
+  <si>
+    <t>Validate that EXTI 2 Works on any logic change</t>
+  </si>
+  <si>
+    <t>Validate that EXTI 1 higher priority than EXTI 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-STM32CUBE IDE 
+2- Proteus Simulation
+3- RCC Driver 
+4- GPIO Driver
+5- LCD Driver
+6- AFIO Driver
+7- NVIC Driver 
+8- EXTI Driver
+</t>
+  </si>
+  <si>
+    <t>Change Switch State Twice</t>
+  </si>
+  <si>
+    <t>Make Change in same time for two exti</t>
+  </si>
+  <si>
+    <t>Display
+"Ana ECU1 Ya Bro"</t>
+  </si>
+  <si>
+    <t>Display
+"Ana ECU2 Ya Bro"</t>
+  </si>
+  <si>
+    <t>Display
+"Ana ECU1 Ya Bro"
+then
+"Ana ECU2 Ya Bro"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+"Ana ECU1 Ya Bro"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+"Ana ECU2 Ya Bro"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+"Ana ECU1 Ya Bro"
+then
+"Ana ECU2 Ya Bro"</t>
+  </si>
+  <si>
+    <t>Unit Test</t>
   </si>
 </sst>
 </file>
@@ -623,16 +693,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -641,7 +711,207 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="202">
+  <dxfs count="222">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2972,10 +3242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB1C29D-A9BC-4A81-B2AF-DC978394A8D6}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3034,7 +3304,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
@@ -3067,10 +3337,10 @@
       <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="13"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
+      <c r="A3" s="14"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -3101,10 +3371,10 @@
       <c r="L3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="14"/>
+      <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
+      <c r="A4" s="14"/>
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -3135,10 +3405,10 @@
       <c r="L4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="14"/>
+      <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
+      <c r="A5" s="14"/>
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -3169,10 +3439,10 @@
       <c r="L5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="14"/>
+      <c r="M5" s="16"/>
     </row>
     <row r="6" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="14"/>
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -3203,7 +3473,7 @@
       <c r="L6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="14"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
@@ -3221,7 +3491,7 @@
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B8" t="s">
@@ -3256,7 +3526,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="14"/>
       <c r="B9" t="s">
         <v>44</v>
       </c>
@@ -3404,7 +3674,7 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>63</v>
       </c>
       <c r="B15" t="s">
@@ -3439,7 +3709,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
+      <c r="A16" s="14"/>
       <c r="B16" t="s">
         <v>66</v>
       </c>
@@ -3472,7 +3742,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
+      <c r="A17" s="14"/>
       <c r="B17" t="s">
         <v>67</v>
       </c>
@@ -3505,7 +3775,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
+      <c r="A18" s="14"/>
       <c r="B18" t="s">
         <v>68</v>
       </c>
@@ -3538,7 +3808,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="14"/>
       <c r="B19" t="s">
         <v>69</v>
       </c>
@@ -3636,7 +3906,7 @@
       <c r="M22" s="5"/>
     </row>
     <row r="23" spans="1:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="13" t="s">
         <v>89</v>
       </c>
       <c r="B23" t="s">
@@ -3668,7 +3938,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="14"/>
       <c r="B24" t="s">
         <v>91</v>
       </c>
@@ -3713,7 +3983,7 @@
       <c r="M25" s="5"/>
     </row>
     <row r="26" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="13" t="s">
         <v>112</v>
       </c>
       <c r="B26" t="s">
@@ -3748,7 +4018,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
+      <c r="A27" s="14"/>
       <c r="B27" t="s">
         <v>99</v>
       </c>
@@ -3781,7 +4051,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
+      <c r="A28" s="14"/>
       <c r="B28" t="s">
         <v>100</v>
       </c>
@@ -3814,7 +4084,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
+      <c r="A29" s="14"/>
       <c r="B29" t="s">
         <v>113</v>
       </c>
@@ -3847,7 +4117,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
+      <c r="A30" s="14"/>
       <c r="B30" t="s">
         <v>117</v>
       </c>
@@ -3880,7 +4150,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
+      <c r="A31" s="14"/>
       <c r="B31" t="s">
         <v>118</v>
       </c>
@@ -3912,8 +4182,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17"/>
+    <row r="32" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
       <c r="B32" t="s">
         <v>119</v>
       </c>
@@ -3945,12 +4215,125 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="2"/>
-      <c r="E33" s="3"/>
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+    </row>
+    <row r="34" spans="1:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I34" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A34:A36"/>
     <mergeCell ref="A26:A32"/>
     <mergeCell ref="M2:M6"/>
     <mergeCell ref="A2:A6"/>
@@ -3959,21 +4342,91 @@
     <mergeCell ref="A23:A24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A1:M1 A7:M7 A10:M10 A2:B2 A3:C6 C6:D6 D4:D5 E2:E6 D2:M3 F4:M6 A8:E8 B9:G9 F8:L9 B11:C11 B15:B19 B21 B23:B24 B26:B34 F26:F32">
-    <cfRule type="cellIs" dxfId="201" priority="267" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="268" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="199" priority="269" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="270" operator="equal">
+  <conditionalFormatting sqref="A1:M1 A7:M7 A10:M10 A2:B2 A3:C6 C6:D6 D4:D5 E2:E6 D2:M3 F4:M6 A8:E8 B9:G9 F8:L9 B11:C11 B15:B19 B21 B23:B24 B26:B32 F26:F32 B34:B36 F34:F36">
+    <cfRule type="cellIs" dxfId="221" priority="287" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="220" priority="288" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="219" priority="289" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="218" priority="290" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
+    <cfRule type="cellIs" dxfId="217" priority="259" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="216" priority="260" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="215" priority="261" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="262" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:H11">
+    <cfRule type="cellIs" dxfId="213" priority="255" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="212" priority="256" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="257" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="210" priority="258" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="209" priority="251" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="208" priority="252" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="207" priority="253" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="206" priority="254" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="cellIs" dxfId="205" priority="247" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="204" priority="248" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="203" priority="249" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="202" priority="250" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11">
+    <cfRule type="cellIs" dxfId="201" priority="243" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="200" priority="244" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="199" priority="245" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="198" priority="246" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:M12">
     <cfRule type="cellIs" dxfId="197" priority="239" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -3987,175 +4440,175 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:H11">
-    <cfRule type="cellIs" dxfId="193" priority="235" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="192" priority="236" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="237" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="238" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="189" priority="231" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="232" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="233" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="186" priority="234" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="185" priority="227" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="228" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="183" priority="229" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="230" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J11">
-    <cfRule type="cellIs" dxfId="181" priority="223" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="180" priority="224" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="225" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="226" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12:M12">
-    <cfRule type="cellIs" dxfId="177" priority="219" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="220" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="221" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="174" priority="222" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="cellIs" dxfId="173" priority="207" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="208" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="209" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="227" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="192" priority="228" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="191" priority="229" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="230" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13 F15:F16">
-    <cfRule type="cellIs" dxfId="169" priority="191" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="192" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="193" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="211" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="188" priority="212" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="187" priority="213" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="186" priority="214" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13 I15:I19">
-    <cfRule type="cellIs" dxfId="165" priority="187" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="188" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="189" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="207" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="184" priority="208" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="183" priority="209" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="182" priority="210" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="161" priority="175" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="176" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="177" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="195" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="180" priority="196" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="179" priority="197" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="178" priority="198" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="157" priority="171" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="172" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="173" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="191" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="192" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="175" priority="193" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="174" priority="194" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="153" priority="167" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="168" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="169" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="187" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="172" priority="188" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="171" priority="189" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="170" priority="190" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="149" priority="163" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="164" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="165" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="183" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="168" priority="184" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="167" priority="185" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="186" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="165" priority="175" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="176" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="163" priority="177" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="162" priority="178" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L13">
+    <cfRule type="cellIs" dxfId="161" priority="171" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="172" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="159" priority="173" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="174" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L11">
+    <cfRule type="cellIs" dxfId="157" priority="167" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="156" priority="168" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="169" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="170" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="cellIs" dxfId="153" priority="163" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="152" priority="164" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="165" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="166" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="cellIs" dxfId="149" priority="159" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="160" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="161" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="162" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:M14">
     <cfRule type="cellIs" dxfId="145" priority="155" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4169,7 +4622,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
+  <conditionalFormatting sqref="A15">
     <cfRule type="cellIs" dxfId="141" priority="151" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4183,7 +4636,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L11">
+  <conditionalFormatting sqref="C15:C19">
     <cfRule type="cellIs" dxfId="137" priority="147" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4197,7 +4650,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
+  <conditionalFormatting sqref="E15:E19">
     <cfRule type="cellIs" dxfId="133" priority="143" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4211,7 +4664,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
+  <conditionalFormatting sqref="G15:H15">
     <cfRule type="cellIs" dxfId="129" priority="139" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4225,77 +4678,77 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:M14">
-    <cfRule type="cellIs" dxfId="125" priority="135" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="136" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="137" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="138" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="121" priority="131" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="132" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="133" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="134" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C19">
-    <cfRule type="cellIs" dxfId="117" priority="127" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="128" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="129" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="130" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15:E19">
-    <cfRule type="cellIs" dxfId="113" priority="123" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="124" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="125" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="126" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G15:H15">
-    <cfRule type="cellIs" dxfId="109" priority="119" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="120" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="121" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="122" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L15:L19">
+    <cfRule type="cellIs" dxfId="125" priority="131" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="132" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="133" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="134" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J15:J19">
+    <cfRule type="cellIs" dxfId="121" priority="127" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="128" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="129" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="130" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15:K19">
+    <cfRule type="cellIs" dxfId="117" priority="123" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="124" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="125" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="126" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:M20">
+    <cfRule type="cellIs" dxfId="113" priority="119" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="120" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="111" priority="121" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="122" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="cellIs" dxfId="109" priority="115" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="116" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="117" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="118" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
     <cfRule type="cellIs" dxfId="105" priority="111" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4309,7 +4762,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J15:J19">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="101" priority="107" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4323,7 +4776,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K15:K19">
+  <conditionalFormatting sqref="I21">
     <cfRule type="cellIs" dxfId="97" priority="103" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4337,7 +4790,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:M20">
+  <conditionalFormatting sqref="J21">
     <cfRule type="cellIs" dxfId="93" priority="99" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4351,7 +4804,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
+  <conditionalFormatting sqref="K21">
     <cfRule type="cellIs" dxfId="89" priority="95" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4365,7 +4818,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="L21">
     <cfRule type="cellIs" dxfId="85" priority="91" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4379,7 +4832,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="A22:M22">
     <cfRule type="cellIs" dxfId="81" priority="87" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4393,7 +4846,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21">
+  <conditionalFormatting sqref="A23">
     <cfRule type="cellIs" dxfId="77" priority="83" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4407,7 +4860,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J21">
+  <conditionalFormatting sqref="C23:C24">
     <cfRule type="cellIs" dxfId="73" priority="79" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4421,96 +4874,96 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="69" priority="75" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="76" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="77" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="78" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L21">
-    <cfRule type="cellIs" dxfId="65" priority="71" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="72" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="73" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="74" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22:M22">
-    <cfRule type="cellIs" dxfId="61" priority="67" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="68" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="69" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="70" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23">
-    <cfRule type="cellIs" dxfId="57" priority="63" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="65" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="66" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23:C24">
-    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="60" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="61" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="62" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E23:E24">
-    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="67" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="68" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="69" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="70" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:I24">
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="66" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:M25">
+    <cfRule type="cellIs" dxfId="64" priority="62" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J23">
+    <cfRule type="cellIs" dxfId="60" priority="58" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J24">
+    <cfRule type="cellIs" dxfId="56" priority="54" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="57" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="cellIs" dxfId="52" priority="50" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24">
+    <cfRule type="cellIs" dxfId="48" priority="46" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="49" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L23">
     <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4524,7 +4977,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J23">
+  <conditionalFormatting sqref="L24">
     <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4538,7 +4991,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24">
+  <conditionalFormatting sqref="A26">
     <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4552,7 +5005,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
+  <conditionalFormatting sqref="C26:C32">
     <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4566,7 +5019,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
+  <conditionalFormatting sqref="E26:E32">
     <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>
@@ -4580,82 +5033,82 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L23">
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L24">
-    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C33">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E33">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
-      <formula>"inProgress"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"onGoing"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>$I$27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:L32">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33:M33">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34:C36">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34:E36">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"inProgress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"onGoing"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J34:L36">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"inProgress"</formula>
     </cfRule>

</xml_diff>